<commit_message>
fix requirements and part of the preprocessing
</commit_message>
<xml_diff>
--- a/Documentation_Reviews.xlsx
+++ b/Documentation_Reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\Bulgaria\SAR-SHIP-DETECTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3EB4DB-D187-4263-8E14-D04054809742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81581D1-2BB1-4127-9343-52DA0FC43A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>last thing to do</t>
+  </si>
+  <si>
+    <t>Steven/Nadia</t>
+  </si>
+  <si>
+    <t>in conflict with row 5 ??</t>
   </si>
 </sst>
 </file>
@@ -525,7 +531,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,6 +562,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -735,7 +747,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -831,24 +843,26 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,10 +1182,10 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1230,7 +1244,7 @@
       <c r="G2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="39"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -1252,7 +1266,7 @@
       <c r="G3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="40"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -1274,9 +1288,7 @@
       <c r="G4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="38" t="s">
-        <v>121</v>
-      </c>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1298,6 +1310,7 @@
       <c r="G5" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -1319,6 +1332,7 @@
       <c r="G6" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -1338,6 +1352,7 @@
       <c r="G7" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -1359,6 +1374,7 @@
       <c r="G8" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -1380,9 +1396,7 @@
       <c r="G9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="38" t="s">
-        <v>121</v>
-      </c>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
@@ -1404,6 +1418,9 @@
       <c r="G10" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="H10" s="33" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
@@ -1425,7 +1442,7 @@
       <c r="G11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="33" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1449,6 +1466,7 @@
       <c r="G12" s="18" t="s">
         <v>43</v>
       </c>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -1470,6 +1488,9 @@
       <c r="G13" s="18" t="s">
         <v>46</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
@@ -1491,6 +1512,7 @@
       <c r="G14" s="18" t="s">
         <v>50</v>
       </c>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
@@ -1512,6 +1534,9 @@
       <c r="G15" s="18" t="s">
         <v>53</v>
       </c>
+      <c r="H15" s="42" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -1533,6 +1558,7 @@
       <c r="G16" s="18" t="s">
         <v>56</v>
       </c>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -1554,7 +1580,7 @@
       <c r="G17" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="33" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2343,22 +2369,22 @@
       <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="34"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
@@ -3169,6 +3195,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="792da008-023a-4535-b591-94dc32feb87f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="59f62bbe-2e25-4bbc-b3d9-76ec598ebb22">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x0101001E7552FD7427C94D9C1A260AEB17A6B2" ma:contentTypeVersion="12" ma:contentTypeDescription="Създаване на нов документ" ma:contentTypeScope="" ma:versionID="0eee8f92f0c94def16b607033ad67c14">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="59f62bbe-2e25-4bbc-b3d9-76ec598ebb22" xmlns:ns3="792da008-023a-4535-b591-94dc32feb87f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e010399ec5a0039dffbd72877db4027a" ns2:_="" ns3:_="">
     <xsd:import namespace="59f62bbe-2e25-4bbc-b3d9-76ec598ebb22"/>
@@ -3369,27 +3415,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="792da008-023a-4535-b591-94dc32feb87f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="59f62bbe-2e25-4bbc-b3d9-76ec598ebb22">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82C94B59-D9CD-4A46-8C75-200A25FAC562}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF8897D-8941-4075-871C-026DCF83A309}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="792da008-023a-4535-b591-94dc32feb87f"/>
+    <ds:schemaRef ds:uri="59f62bbe-2e25-4bbc-b3d9-76ec598ebb22"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B061121-2C63-4293-B0DE-220AEF1680EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3408,25 +3453,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF8897D-8941-4075-871C-026DCF83A309}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="792da008-023a-4535-b591-94dc32feb87f"/>
-    <ds:schemaRef ds:uri="59f62bbe-2e25-4bbc-b3d9-76ec598ebb22"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82C94B59-D9CD-4A46-8C75-200A25FAC562}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{4a18cb8b-b568-4ac9-8854-51740db0235a}" enabled="1" method="Standard" siteId="{60c58ca1-7962-4dfa-8d08-86343a279fd6}" removed="0"/>

</xml_diff>